<commit_message>
Player Jump, UI Click
</commit_message>
<xml_diff>
--- a/210213 - BTBB Fmod/AudioSheet.xlsx
+++ b/210213 - BTBB Fmod/AudioSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\Audio 4 Games\GameJam\BTBB\BringTheBandBack\210213 - BTBB Fmod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB6B9E-63F4-45BC-87D6-F994F0DD5530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE89E48D-176B-4C24-8345-170736E05676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2616" yWindow="2628" windowWidth="17280" windowHeight="9024" xr2:uid="{E04EF97F-7E8B-4B9D-B339-6A4999538D1B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>event:/Atmos/Haunting</t>
   </si>
@@ -191,13 +191,19 @@
     <t>event:/Vocals/Scream</t>
   </si>
   <si>
-    <t>Moved</t>
-  </si>
-  <si>
     <t>event:/Guitar/Attack</t>
   </si>
   <si>
     <t>event:/Objects/Coin/Coin</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>moved</t>
   </si>
 </sst>
 </file>
@@ -213,12 +219,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -233,9 +251,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,23 +570,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE1E26B-AF1F-4721-93C0-14DBB81FF15F}">
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
@@ -582,8 +606,12 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +625,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -617,7 +646,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -637,7 +667,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -657,7 +688,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -677,7 +709,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -688,7 +721,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -699,7 +733,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
@@ -710,7 +745,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
@@ -718,7 +754,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
@@ -738,7 +775,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -758,7 +796,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -766,7 +805,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
@@ -774,9 +814,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -795,6 +836,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
@@ -803,6 +845,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
@@ -823,6 +866,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
@@ -831,6 +875,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
@@ -839,6 +884,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
@@ -847,6 +893,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
@@ -855,6 +902,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
@@ -875,6 +923,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
@@ -895,6 +944,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -906,6 +956,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
@@ -926,6 +977,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
@@ -934,17 +986,19 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>52</v>
-      </c>
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
@@ -953,6 +1007,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
       <c r="B30" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
piano rolling, death and damage sounds
</commit_message>
<xml_diff>
--- a/210213 - BTBB Fmod/AudioSheet.xlsx
+++ b/210213 - BTBB Fmod/AudioSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\Audio 4 Games\GameJam\BTBB\BringTheBandBack\210213 - BTBB Fmod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36CFDFD-0BC2-4CC2-A3DE-0B4C98CF0F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9415684F-D668-42A1-9A18-A2DB8B53F311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{E04EF97F-7E8B-4B9D-B339-6A4999538D1B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E04EF97F-7E8B-4B9D-B339-6A4999538D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>chords</t>
   </si>
   <si>
-    <t>event:/Piano/Rolling</t>
-  </si>
-  <si>
     <t>event:/Piano/Spawn</t>
   </si>
   <si>
@@ -203,7 +200,10 @@
     <t>Implemented</t>
   </si>
   <si>
-    <t>moved</t>
+    <t>needs to be re implemented</t>
+  </si>
+  <si>
+    <t>event:/Object/Piano/Rolling</t>
   </si>
 </sst>
 </file>
@@ -572,14 +572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE1E26B-AF1F-4721-93C0-14DBB81FF15F}">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -589,7 +589,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -607,7 +607,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -868,7 +868,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -877,40 +877,40 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
@@ -919,19 +919,19 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -940,25 +940,25 @@
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -973,34 +973,34 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -1009,7 +1009,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Very Buggy Piano Sound Implementatino
</commit_message>
<xml_diff>
--- a/210213 - BTBB Fmod/AudioSheet.xlsx
+++ b/210213 - BTBB Fmod/AudioSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\Audio 4 Games\GameJam\BTBB\BringTheBandBack\210213 - BTBB Fmod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9415684F-D668-42A1-9A18-A2DB8B53F311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC9B434-95E7-44B0-9B93-C3FC64EF7C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E04EF97F-7E8B-4B9D-B339-6A4999538D1B}"/>
   </bookViews>
@@ -191,19 +191,19 @@
     <t>event:/Guitar/Attack</t>
   </si>
   <si>
-    <t>event:/Objects/Coin/Coin</t>
-  </si>
-  <si>
     <t>Created</t>
   </si>
   <si>
     <t>Implemented</t>
   </si>
   <si>
-    <t>needs to be re implemented</t>
-  </si>
-  <si>
     <t>event:/Object/Piano/Rolling</t>
+  </si>
+  <si>
+    <t>event:/Objects/Pickups/Note</t>
+  </si>
+  <si>
+    <t>Buggy</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -251,11 +257,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +596,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -607,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,12 +873,18 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -986,16 +999,17 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" t="s">
         <v>55</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>

</xml_diff>